<commit_message>
Verificando o tamanho dos logs de cada época
</commit_message>
<xml_diff>
--- a/sniper/tools/results_cpu2017.xlsx
+++ b/sniper/tools/results_cpu2017.xlsx
@@ -729,64 +729,64 @@
         <v>1574015000</v>
       </c>
       <c r="C6">
-        <v>5450400</v>
+        <v>1753042400</v>
       </c>
       <c r="D6">
-        <v>5398200</v>
+        <v>1747289800</v>
       </c>
       <c r="E6">
         <v>0.16</v>
       </c>
       <c r="F6">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="G6">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="H6">
         <v>26472269</v>
       </c>
       <c r="I6">
-        <v>6998</v>
+        <v>28221816</v>
       </c>
       <c r="J6">
-        <v>6916</v>
+        <v>28219798</v>
       </c>
       <c r="K6">
         <v>9728712</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>9719732</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>9719861</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>6998</v>
+        <v>18502084</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>9719861</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
-        <v>109</v>
+        <v>289095</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>151872</v>
       </c>
       <c r="T6">
         <v>0</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>848</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1953,64 +1953,64 @@
         <v>811261600</v>
       </c>
       <c r="C24">
-        <v>1117800</v>
+        <v>836215000</v>
       </c>
       <c r="D24">
-        <v>1123000</v>
+        <v>836629600</v>
       </c>
       <c r="E24">
         <v>0.23</v>
       </c>
       <c r="F24">
-        <v>0.03</v>
+        <v>0.22</v>
       </c>
       <c r="G24">
-        <v>0.03</v>
+        <v>0.22</v>
       </c>
       <c r="H24">
         <v>18962287</v>
       </c>
       <c r="I24">
-        <v>3461</v>
+        <v>18999065</v>
       </c>
       <c r="J24">
-        <v>3461</v>
+        <v>19002462</v>
       </c>
       <c r="K24">
         <v>9205944</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>9238432</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>9242938</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24">
-        <v>3461</v>
+        <v>9760633</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>9242938</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
-        <v>54</v>
+        <v>152509</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>144420</v>
       </c>
       <c r="T24">
         <v>0</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>1162</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="25" spans="1:22">

</xml_diff>